<commit_message>
Updated README and multitenancy calculations
</commit_message>
<xml_diff>
--- a/PowerBI_Embedded_Calculator.xlsx
+++ b/PowerBI_Embedded_Calculator.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cesanu\OneDrive - Microsoft\DOCS\AMDOCS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cesanu\OneDrive - Microsoft\DOCS\PBI_Embedded\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="311" documentId="8_{71698348-278B-4BA5-833A-E4524B28830D}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{9F71E5C4-B77B-4C70-B28A-22ED02B5CEA2}"/>
+  <xr:revisionPtr revIDLastSave="326" documentId="8_{71698348-278B-4BA5-833A-E4524B28830D}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{7E58DBDE-153D-4BFA-8281-B3958D64B811}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{CA052A36-0C6A-4A41-B543-611774494988}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{CA052A36-0C6A-4A41-B543-611774494988}"/>
   </bookViews>
   <sheets>
     <sheet name="Calculator" sheetId="1" r:id="rId1"/>
@@ -190,9 +190,6 @@
     <t>P5</t>
   </si>
   <si>
-    <t>Parallel Refreshes Per Capacity</t>
-  </si>
-  <si>
     <t>Max Capacity Costs</t>
   </si>
   <si>
@@ -235,9 +232,6 @@
     <t># Number of visuals or other elements that affect renders</t>
   </si>
   <si>
-    <t>Active Parallel Models</t>
-  </si>
-  <si>
     <t>Capcity Type By Active Model Memory Consumption</t>
   </si>
   <si>
@@ -251,6 +245,12 @@
   </si>
   <si>
     <t># Models that are loaded into memory at the same time</t>
+  </si>
+  <si>
+    <t>Active Parallel Models Per Tenant</t>
+  </si>
+  <si>
+    <t>Parallel Refreshes Per Tenant</t>
   </si>
 </sst>
 </file>
@@ -542,10 +542,10 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="4" fontId="3" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -557,7 +557,7 @@
     <xf numFmtId="4" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -622,9 +622,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>2484058</xdr:colOff>
+      <xdr:colOff>2480248</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>1530350</xdr:rowOff>
+      <xdr:rowOff>1528445</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -977,26 +977,26 @@
   <dimension ref="A1:O36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="58.90625" customWidth="1"/>
-    <col min="2" max="2" width="28.54296875" customWidth="1"/>
+    <col min="1" max="1" width="58.85546875" customWidth="1"/>
+    <col min="2" max="2" width="28.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="127.75" customHeight="1" x14ac:dyDescent="1">
+    <row r="1" spans="1:15" ht="127.7" customHeight="1" x14ac:dyDescent="0.7">
       <c r="B1" s="32" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" s="30" customFormat="1" ht="26" x14ac:dyDescent="0.6">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" s="30" customFormat="1" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A5" s="30" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="6" spans="1:15" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:15" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A6" s="23" t="s">
         <v>0</v>
       </c>
@@ -1004,7 +1004,7 @@
         <v>9.99</v>
       </c>
     </row>
-    <row r="7" spans="1:15" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:15" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A7" s="23" t="s">
         <v>1</v>
       </c>
@@ -1012,10 +1012,10 @@
         <v>1</v>
       </c>
       <c r="D7" s="29" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" ht="18.5" x14ac:dyDescent="0.45">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A8" s="23" t="s">
         <v>2</v>
       </c>
@@ -1023,10 +1023,10 @@
         <v>1</v>
       </c>
       <c r="D8" s="29" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" ht="18.5" x14ac:dyDescent="0.45">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A9" s="23" t="s">
         <v>3</v>
       </c>
@@ -1034,10 +1034,10 @@
         <v>15</v>
       </c>
       <c r="D9" s="29" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15" ht="18.5" x14ac:dyDescent="0.45">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A10" s="23" t="s">
         <v>4</v>
       </c>
@@ -1045,10 +1045,10 @@
         <v>20</v>
       </c>
       <c r="D10" s="29" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15" ht="18.5" x14ac:dyDescent="0.45">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A11" s="23" t="s">
         <v>5</v>
       </c>
@@ -1056,10 +1056,10 @@
         <v>10</v>
       </c>
       <c r="D11" s="29" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="12" spans="1:15" ht="18.5" x14ac:dyDescent="0.45">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A12" s="23" t="s">
         <v>23</v>
       </c>
@@ -1067,10 +1067,10 @@
         <v>11</v>
       </c>
       <c r="D12" s="29" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="13" spans="1:15" ht="18.5" x14ac:dyDescent="0.45">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A13" s="23" t="s">
         <v>40</v>
       </c>
@@ -1079,38 +1079,38 @@
       </c>
       <c r="D13" s="29"/>
     </row>
-    <row r="14" spans="1:15" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:15" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A14" s="23" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="B14" s="23">
         <v>1</v>
       </c>
       <c r="D14" s="29" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A15" s="23" t="s">
         <v>72</v>
-      </c>
-    </row>
-    <row r="15" spans="1:15" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A15" s="23" t="s">
-        <v>52</v>
       </c>
       <c r="B15" s="23">
         <v>1</v>
       </c>
       <c r="D15" s="29" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="O15" s="20"/>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="D16" s="29"/>
     </row>
-    <row r="17" spans="1:15" s="31" customFormat="1" ht="26" x14ac:dyDescent="0.6">
+    <row r="17" spans="1:15" s="31" customFormat="1" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A17" s="31" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="18" spans="1:15" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:15" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A18" s="23" t="s">
         <v>24</v>
       </c>
@@ -1121,7 +1121,7 @@
       <c r="D18" s="29"/>
       <c r="O18" s="21"/>
     </row>
-    <row r="19" spans="1:15" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:15" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A19" s="23" t="s">
         <v>25</v>
       </c>
@@ -1131,7 +1131,7 @@
       </c>
       <c r="D19" s="29"/>
     </row>
-    <row r="20" spans="1:15" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:15" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A20" s="23" t="s">
         <v>41</v>
       </c>
@@ -1141,7 +1141,7 @@
       </c>
       <c r="D20" s="29"/>
     </row>
-    <row r="21" spans="1:15" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:15" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A21" s="23" t="s">
         <v>42</v>
       </c>
@@ -1151,36 +1151,36 @@
       </c>
       <c r="D21" s="29"/>
     </row>
-    <row r="22" spans="1:15" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:15" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A22" s="23" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B22" s="23" t="str">
-        <f>LOOKUP(2,1/(Metadata!$I$2:'Metadata'!$I$8&lt;=(B14+B15)*B13)/(Metadata!$J$2:'Metadata'!$J$8&gt;=(B14+B15)*B13),Metadata!$A$2:'Metadata'!$A$8)</f>
+        <f>LOOKUP(2,1/(Metadata!$I$2:'Metadata'!$I$8&lt;=IF(B12="Yes",B7,1)*(B14+B15)*B13)/(Metadata!$J$2:'Metadata'!$J$8&gt;=IF(B12="Yes",B7,1)*(B14+B15)*B13),Metadata!$A$2:'Metadata'!$A$8)</f>
         <v>A1</v>
       </c>
       <c r="D22" s="29"/>
     </row>
-    <row r="23" spans="1:15" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:15" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A23" s="23" t="s">
         <v>43</v>
       </c>
       <c r="B23" s="23" t="str">
-        <f>LOOKUP(2,1/(Metadata!$C$31:'Metadata'!$C$36&lt;=B15)/(Metadata!$D$31:'Metadata'!$D$36&gt;=B15),Metadata!$A$31:'Metadata'!$A$36)</f>
+        <f>LOOKUP(2,1/(Metadata!$C$31:'Metadata'!$C$36&lt;=IF(B12="Yes",B7,1)*B15)/(Metadata!$D$31:'Metadata'!$D$36&gt;=IF(B12="Yes",B7,1)*B15),Metadata!$A$31:'Metadata'!$A$36)</f>
         <v>A1</v>
       </c>
       <c r="D23" s="29"/>
     </row>
-    <row r="24" spans="1:15" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:15" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A24" s="33" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B24" s="23"/>
       <c r="D24" s="29"/>
     </row>
-    <row r="25" spans="1:15" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:15" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A25" s="23" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B25" s="23" t="str">
         <f t="array" ref="B25">"A"&amp;MAX((0&amp;SUBSTITUTE(B20:B23,"A",""))+0)</f>
@@ -1188,9 +1188,9 @@
       </c>
       <c r="D25" s="29"/>
     </row>
-    <row r="26" spans="1:15" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:15" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A26" s="23" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B26" s="24">
         <f>LOOKUP(B25,Metadata!$A$2:'Metadata'!$A$8,Metadata!$F$2:'Metadata'!$F$8)</f>
@@ -1198,15 +1198,15 @@
       </c>
       <c r="D26" s="29"/>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="D27" s="29"/>
     </row>
-    <row r="28" spans="1:15" s="31" customFormat="1" ht="26" x14ac:dyDescent="0.6">
+    <row r="28" spans="1:15" s="31" customFormat="1" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A28" s="31" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="29" spans="1:15" ht="21" x14ac:dyDescent="0.5">
+    <row r="29" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A29" s="25" t="s">
         <v>26</v>
       </c>
@@ -1216,7 +1216,7 @@
       </c>
       <c r="D29" s="29"/>
     </row>
-    <row r="30" spans="1:15" ht="21" x14ac:dyDescent="0.5">
+    <row r="30" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A30" s="25" t="s">
         <v>27</v>
       </c>
@@ -1225,10 +1225,10 @@
         <v>9.99</v>
       </c>
       <c r="D30" s="29" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="31" spans="1:15" ht="21" x14ac:dyDescent="0.5">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A31" s="25" t="s">
         <v>28</v>
       </c>
@@ -1237,7 +1237,7 @@
         <v>735.92</v>
       </c>
     </row>
-    <row r="35" spans="1:2" s="13" customFormat="1" ht="33.5" x14ac:dyDescent="0.75">
+    <row r="35" spans="1:2" s="13" customFormat="1" ht="33.75" x14ac:dyDescent="0.5">
       <c r="A35" s="27" t="s">
         <v>33</v>
       </c>
@@ -1246,9 +1246,9 @@
         <v>845.81</v>
       </c>
     </row>
-    <row r="36" spans="1:2" ht="33.5" x14ac:dyDescent="0.75">
+    <row r="36" spans="1:2" ht="33.75" x14ac:dyDescent="0.5">
       <c r="A36" s="27" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B36" s="28">
         <f>B35*12</f>
@@ -1275,17 +1275,17 @@
       <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.36328125" customWidth="1"/>
-    <col min="2" max="2" width="19.1796875" customWidth="1"/>
-    <col min="3" max="3" width="23.08984375" customWidth="1"/>
-    <col min="4" max="4" width="15.36328125" customWidth="1"/>
-    <col min="5" max="5" width="12.81640625" customWidth="1"/>
+    <col min="1" max="1" width="12.42578125" customWidth="1"/>
+    <col min="2" max="2" width="19.140625" customWidth="1"/>
+    <col min="3" max="3" width="23.140625" customWidth="1"/>
+    <col min="4" max="4" width="15.42578125" customWidth="1"/>
+    <col min="5" max="5" width="12.85546875" customWidth="1"/>
     <col min="6" max="6" width="19" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="32" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:10" ht="27.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
         <v>6</v>
       </c>
@@ -1296,7 +1296,7 @@
         <v>8</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E1" s="6" t="s">
         <v>9</v>
@@ -1311,13 +1311,13 @@
         <v>21</v>
       </c>
       <c r="I1" s="7" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="J1" s="7" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>10</v>
       </c>
@@ -1350,7 +1350,7 @@
         <v>3072</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>13</v>
       </c>
@@ -1380,11 +1380,11 @@
         <v>3073</v>
       </c>
       <c r="J3">
-        <f t="shared" ref="J3:J8" si="0">D3*1024</f>
+        <f t="shared" ref="J3:J7" si="0">D3*1024</f>
         <v>5120</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>14</v>
       </c>
@@ -1418,7 +1418,7 @@
         <v>10240</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>16</v>
       </c>
@@ -1452,7 +1452,7 @@
         <v>25600</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>17</v>
       </c>
@@ -1486,7 +1486,7 @@
         <v>51200</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
         <v>18</v>
       </c>
@@ -1520,7 +1520,7 @@
         <v>102400</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="12" t="s">
         <v>29</v>
       </c>
@@ -1545,10 +1545,10 @@
         <v>10240000</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="15" spans="1:10" ht="67" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="14" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="15" spans="1:10" ht="67.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="18" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B15" s="18" t="s">
         <v>38</v>
@@ -1558,7 +1558,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="17.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="16" spans="1:10" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="22"/>
       <c r="B16" s="22" t="s">
         <v>10</v>
@@ -1571,7 +1571,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="17.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="17" spans="1:4" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="22"/>
       <c r="B17" s="22" t="s">
         <v>13</v>
@@ -1585,7 +1585,7 @@
         <v>614</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="17.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="18" spans="1:4" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="22"/>
       <c r="B18" s="22" t="s">
         <v>14</v>
@@ -1599,7 +1599,7 @@
         <v>1228</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="17.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:4" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="16" t="s">
         <v>35</v>
       </c>
@@ -1615,7 +1615,7 @@
         <v>3072</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="17.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:4" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="16" t="s">
         <v>36</v>
       </c>
@@ -1631,7 +1631,7 @@
         <v>6144</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="17.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:4" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="16" t="s">
         <v>37</v>
       </c>
@@ -1647,8 +1647,8 @@
         <v>10240</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="15" thickTop="1" x14ac:dyDescent="0.35"/>
-    <row r="30" spans="1:4" ht="50" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="22" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="30" spans="1:4" ht="50.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A30" s="14" t="s">
         <v>34</v>
       </c>
@@ -1660,7 +1660,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:4" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="15" t="s">
         <v>10</v>
       </c>
@@ -1674,7 +1674,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:4" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="15" t="s">
         <v>13</v>
       </c>
@@ -1688,7 +1688,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:4" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="15" t="s">
         <v>14</v>
       </c>
@@ -1702,7 +1702,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:4" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="15" t="s">
         <v>16</v>
       </c>
@@ -1716,7 +1716,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:4" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="15" t="s">
         <v>17</v>
       </c>
@@ -1730,7 +1730,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="36" spans="1:4" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="15" t="s">
         <v>18</v>
       </c>
@@ -1744,7 +1744,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="37" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="37" spans="1:4" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="15" t="s">
         <v>46</v>
       </c>
@@ -1758,7 +1758,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="38" spans="1:4" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="15" t="s">
         <v>47</v>
       </c>
@@ -1772,7 +1772,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="39" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="39" spans="1:4" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="15" t="s">
         <v>48</v>
       </c>
@@ -1786,7 +1786,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="40" spans="1:4" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="15" t="s">
         <v>35</v>
       </c>
@@ -1800,7 +1800,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="41" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="41" spans="1:4" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="15" t="s">
         <v>36</v>
       </c>
@@ -1814,7 +1814,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="42" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="42" spans="1:4" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="15" t="s">
         <v>49</v>
       </c>
@@ -1828,7 +1828,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="43" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="43" spans="1:4" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="15" t="s">
         <v>50</v>
       </c>
@@ -1842,7 +1842,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="44" spans="1:4" ht="16.5" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A44" s="15" t="s">
         <v>51</v>
       </c>

</xml_diff>